<commit_message>
Finished Design thinking section
waiting for comments
</commit_message>
<xml_diff>
--- a/UserStudies/tempSensing/peltiers/AllData.xlsx
+++ b/UserStudies/tempSensing/peltiers/AllData.xlsx
@@ -167,9 +167,6 @@
     <t>Average time per turn</t>
   </si>
   <si>
-    <t>Average time VS Feedback</t>
-  </si>
-  <si>
     <t>Feedback first</t>
   </si>
   <si>
@@ -200,6 +197,10 @@
   </si>
   <si>
     <t>Average time of feedback  Vs no feedback</t>
+  </si>
+  <si>
+    <t>Average total time when feedback
+was first or second</t>
   </si>
 </sst>
 </file>
@@ -264,13 +265,13 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -646,11 +647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136873472"/>
-        <c:axId val="136875008"/>
+        <c:axId val="127846272"/>
+        <c:axId val="127847808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136873472"/>
+        <c:axId val="127846272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136875008"/>
+        <c:crossAx val="127847808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136875008"/>
+        <c:axId val="127847808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136873472"/>
+        <c:crossAx val="127846272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,11 +737,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="User12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,31 +749,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user07" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user10" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user11" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user09" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tito03" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user07" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user11" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="User12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,7 +1066,7 @@
   <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,9 +1080,9 @@
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="8" width="2" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1105,7 +1106,7 @@
         <v>162.69293900100001</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2">
         <f>AVERAGE(A2:A13,A18:A29,A34:A45,A50:A61,A66:A77,A82:A93,A98:A109,A114:A125,A130:A141,A146:A157)</f>
@@ -1258,12 +1259,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
@@ -1275,10 +1276,10 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1677,17 +1678,17 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="33" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="33" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>41918</v>
       </c>
@@ -1698,11 +1699,11 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -1716,14 +1717,14 @@
         <v>26.879466001000001</v>
       </c>
       <c r="I34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1741,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J35" s="4">
         <f>AVERAGE(C18:C29,C50:C61,C82:C93,C98:C109,C114:C125,C130:C141)</f>
@@ -1765,7 +1766,7 @@
         <v>40.428919999000001</v>
       </c>
       <c r="I36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J36" s="4">
         <f>AVERAGE(C2:C13,C34:C45,C66:C77,C146:C157)</f>
@@ -1801,12 +1802,12 @@
       <c r="C38" s="4">
         <v>32.680228999999997</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
+      <c r="I38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -1820,14 +1821,14 @@
         <v>16.031256999</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="K39" s="7"/>
       <c r="L39" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1845,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J40" s="4">
         <f>AVERAGE(C24:C29,C56:C61,C88:C93,C104:C109,C120:C125,C136:C141)</f>
@@ -1870,7 +1871,7 @@
       </c>
       <c r="D41" s="1"/>
       <c r="I41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J41" s="4">
         <f>AVERAGE(C2:C7,C34:C39,C66:C71,C146:C151)</f>
@@ -1908,12 +1909,12 @@
         <v>25.191258999999999</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="I43" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
+      <c r="I43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1928,14 +1929,14 @@
       </c>
       <c r="D44" s="1"/>
       <c r="I44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -1951,7 +1952,7 @@
       </c>
       <c r="D45" s="1"/>
       <c r="I45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J45" s="4">
         <f>AVERAGE(C24:C29,C56:C61,C88:C93,C104:C109,C120:C125,C136:C141)</f>
@@ -1974,7 +1975,7 @@
       </c>
       <c r="D46" s="1"/>
       <c r="I46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J46" s="4">
         <f>AVERAGE(C8:C13,C40:C45,C72:C77,C146:C151)</f>
@@ -1982,28 +1983,28 @@
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="8">
-        <f>AVERAGE(A8:A13,A40:A45,A72:A77,A146:A151)</f>
+        <f>AVERAGE(A8:A13,A40:A45,A72:A77,A152:A157)</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I48" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
+      <c r="I48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2016,14 +2017,14 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="K49" s="7"/>
       <c r="L49" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2039,7 +2040,7 @@
       </c>
       <c r="D50" s="1"/>
       <c r="I50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J50" s="4">
         <f>AVERAGE(C114:C119,C130:C135,C8:C13,C18:C23,C40:C45,C50:C55,C72:C77,C82:C87,C98:C103,C152:C157)</f>
@@ -2064,7 +2065,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="I51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J51" s="4">
         <f>AVERAGE(C120:C125,C136:C141,C2:C7,C24:C29,C34:C39,C56:C61,C66:C71,C88:C93,C104:C109,C146:C151)</f>
@@ -2222,15 +2223,15 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="10">
@@ -2409,15 +2410,15 @@
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" s="10">
@@ -2596,15 +2597,15 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
@@ -2781,16 +2782,16 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
@@ -3176,16 +3177,16 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
-      <c r="G143" s="11"/>
-      <c r="H143" s="11"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="10">
@@ -3365,19 +3366,28 @@
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="11"/>
-      <c r="C159" s="11"/>
-      <c r="D159" s="11"/>
-      <c r="E159" s="11"/>
-      <c r="F159" s="11"/>
-      <c r="G159" s="11"/>
-      <c r="H159" s="11"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A143:H143"/>
+    <mergeCell ref="A129:H129"/>
+    <mergeCell ref="A127:H127"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A111:H111"/>
     <mergeCell ref="A159:H159"/>
     <mergeCell ref="A145:H145"/>
     <mergeCell ref="I17:J17"/>
@@ -3391,18 +3401,9 @@
     <mergeCell ref="B65:H65"/>
     <mergeCell ref="B79:H79"/>
     <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A97:H97"/>
-    <mergeCell ref="A111:H111"/>
     <mergeCell ref="I43:L43"/>
     <mergeCell ref="I38:L38"/>
     <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A143:H143"/>
-    <mergeCell ref="A129:H129"/>
-    <mergeCell ref="A127:H127"/>
-    <mergeCell ref="I48:L48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
time for first trial of defense
</commit_message>
<xml_diff>
--- a/UserStudies/tempSensing/peltiers/AllData.xlsx
+++ b/UserStudies/tempSensing/peltiers/AllData.xlsx
@@ -176,10 +176,6 @@
     <t>Average of correct</t>
   </si>
   <si>
-    <t>Average time of last 6 
-with feedback first Vs Second</t>
-  </si>
-  <si>
     <t>Average time of no feedback
 with feedback first Vs Second</t>
   </si>
@@ -201,6 +197,9 @@
   <si>
     <t>Average total time when feedback
 was first or second</t>
+  </si>
+  <si>
+    <t>Time and Accuracy of the last 6 turns, with and without feedback</t>
   </si>
 </sst>
 </file>
@@ -270,11 +269,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,11 +646,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127846272"/>
-        <c:axId val="127847808"/>
+        <c:axId val="125905536"/>
+        <c:axId val="125915520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127846272"/>
+        <c:axId val="125905536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +659,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127847808"/>
+        <c:crossAx val="125915520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127847808"/>
+        <c:axId val="125915520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127846272"/>
+        <c:crossAx val="125905536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -737,11 +736,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user09" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,31 +748,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tito03" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user07" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="User12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user10" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user11" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user09" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tito03" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="User12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,8 +1697,8 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="11" t="s">
-        <v>14</v>
+      <c r="I33" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -1717,14 +1716,14 @@
         <v>26.879466001000001</v>
       </c>
       <c r="I34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1802,12 +1801,12 @@
       <c r="C38" s="4">
         <v>32.680228999999997</v>
       </c>
-      <c r="I38" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
+      <c r="I38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -1821,14 +1820,14 @@
         <v>16.031256999</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="K39" s="7"/>
       <c r="L39" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1909,12 +1908,12 @@
         <v>25.191258999999999</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="I43" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
+      <c r="I43" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1929,14 +1928,14 @@
       </c>
       <c r="D44" s="1"/>
       <c r="I44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -1952,7 +1951,7 @@
       </c>
       <c r="D45" s="1"/>
       <c r="I45" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J45" s="4">
         <f>AVERAGE(C24:C29,C56:C61,C88:C93,C104:C109,C120:C125,C136:C141)</f>
@@ -1975,11 +1974,11 @@
       </c>
       <c r="D46" s="1"/>
       <c r="I46" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J46" s="4">
-        <f>AVERAGE(C8:C13,C40:C45,C72:C77,C146:C151)</f>
-        <v>50.221083999999998</v>
+        <f>AVERAGE(C8:C13,C40:C45,C72:C77,C152:C157)</f>
+        <v>45.95467120833333</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="8">
@@ -1999,12 +1998,12 @@
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
+      <c r="I48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2017,14 +2016,14 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="K49" s="7"/>
       <c r="L49" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2040,7 +2039,7 @@
       </c>
       <c r="D50" s="1"/>
       <c r="I50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J50" s="4">
         <f>AVERAGE(C114:C119,C130:C135,C8:C13,C18:C23,C40:C45,C50:C55,C72:C77,C82:C87,C98:C103,C152:C157)</f>
@@ -2065,7 +2064,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="I51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J51" s="4">
         <f>AVERAGE(C120:C125,C136:C141,C2:C7,C24:C29,C34:C39,C56:C61,C66:C71,C88:C93,C104:C109,C146:C151)</f>
@@ -2979,16 +2978,16 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12"/>
-      <c r="G127" s="12"/>
-      <c r="H127" s="12"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
+      <c r="G127" s="11"/>
+      <c r="H127" s="11"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="10">
@@ -3379,15 +3378,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A143:H143"/>
-    <mergeCell ref="A129:H129"/>
-    <mergeCell ref="A127:H127"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A97:H97"/>
-    <mergeCell ref="A111:H111"/>
     <mergeCell ref="A159:H159"/>
     <mergeCell ref="A145:H145"/>
     <mergeCell ref="I17:J17"/>
@@ -3404,6 +3394,15 @@
     <mergeCell ref="I43:L43"/>
     <mergeCell ref="I38:L38"/>
     <mergeCell ref="A113:H113"/>
+    <mergeCell ref="A143:H143"/>
+    <mergeCell ref="A129:H129"/>
+    <mergeCell ref="A127:H127"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A111:H111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
After correction of trial presentation
</commit_message>
<xml_diff>
--- a/UserStudies/tempSensing/peltiers/AllData.xlsx
+++ b/UserStudies/tempSensing/peltiers/AllData.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="16">
   <si>
     <t>RIGHT</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Time and Accuracy of the last 6 turns, with and without feedback</t>
+  </si>
+  <si>
+    <t>Correlation</t>
   </si>
 </sst>
 </file>
@@ -269,11 +272,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,11 +649,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="125905536"/>
-        <c:axId val="125915520"/>
+        <c:axId val="86046976"/>
+        <c:axId val="86056960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125905536"/>
+        <c:axId val="86046976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125915520"/>
+        <c:crossAx val="86056960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125915520"/>
+        <c:axId val="86056960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +681,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125905536"/>
+        <c:crossAx val="86046976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,11 +739,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user09" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user10" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,31 +751,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user11" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tito03" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user07" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user09" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="User12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user10" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user01" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user11" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user08" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user06" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1064,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,6 +1689,17 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="4">
+        <f>CORREL(I18:I29,J18:J29)</f>
+        <v>-0.58259696849646969</v>
+      </c>
+      <c r="K31" s="4">
+        <f>CORREL(I18:I29,K18:K29)</f>
+        <v>-0.33307845149748194</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
@@ -1697,7 +1711,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J33" s="9"/>
@@ -1801,12 +1815,12 @@
       <c r="C38" s="4">
         <v>32.680228999999997</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -1908,12 +1922,12 @@
         <v>25.191258999999999</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="I43" s="12" t="s">
+      <c r="I43" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1998,12 +2012,12 @@
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I48" s="12" t="s">
+      <c r="I48" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2978,16 +2992,16 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="10">
@@ -3378,6 +3392,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A143:H143"/>
+    <mergeCell ref="A129:H129"/>
+    <mergeCell ref="A127:H127"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A111:H111"/>
     <mergeCell ref="A159:H159"/>
     <mergeCell ref="A145:H145"/>
     <mergeCell ref="I17:J17"/>
@@ -3394,15 +3417,6 @@
     <mergeCell ref="I43:L43"/>
     <mergeCell ref="I38:L38"/>
     <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A143:H143"/>
-    <mergeCell ref="A129:H129"/>
-    <mergeCell ref="A127:H127"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A97:H97"/>
-    <mergeCell ref="A111:H111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>